<commit_message>
add count project feature
</commit_message>
<xml_diff>
--- a/public/excel/score.xlsx
+++ b/public/excel/score.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="255" windowWidth="15480" windowHeight="8415" tabRatio="725"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="15480" windowHeight="8415" tabRatio="725" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ใบกรอกคะแนนPP-mid" sheetId="10" r:id="rId1"/>
@@ -213,13 +213,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="187" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -232,7 +232,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -240,7 +240,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -304,7 +304,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -340,7 +340,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -739,23 +739,23 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="187" fontId="11" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="11" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="11" fillId="3" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="16" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="16" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -763,31 +763,31 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="3" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="19" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="19" fillId="3" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="19" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -795,23 +795,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="19" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="19" fillId="3" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="19" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1151,24 +1151,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K715"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" style="1" customWidth="1"/>
-    <col min="7" max="10" width="13.375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="13.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="3" customWidth="1"/>
     <col min="12" max="12" width="8" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
     <col min="15" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
@@ -6059,12 +6059,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="15.625" style="1" customWidth="1"/>
-    <col min="7" max="11" width="13.375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5703125" style="1" customWidth="1"/>
+    <col min="7" max="11" width="13.42578125" style="3" customWidth="1"/>
     <col min="12" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
@@ -10488,25 +10488,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V658"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.875" style="1" customWidth="1"/>
-    <col min="5" max="7" width="15.625" style="1" customWidth="1"/>
-    <col min="8" max="17" width="13.375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="6.375" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="17" width="13.42578125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" style="3" hidden="1" customWidth="1"/>
     <col min="19" max="21" width="8" style="1" customWidth="1"/>
-    <col min="22" max="22" width="15.625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" style="1" customWidth="1"/>
     <col min="23" max="23" width="8" style="1" customWidth="1"/>
-    <col min="24" max="24" width="17.75" style="1" customWidth="1"/>
-    <col min="25" max="25" width="14.875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" style="1" customWidth="1"/>
     <col min="26" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
@@ -10568,7 +10568,7 @@
       </c>
       <c r="R2" s="36"/>
     </row>
-    <row r="3" spans="1:22" ht="102.75">
+    <row r="3" spans="1:22" ht="178.5">
       <c r="A3" s="78" t="s">
         <v>38</v>
       </c>
@@ -12423,533 +12423,632 @@
       <c r="P92" s="74"/>
       <c r="Q92" s="74"/>
     </row>
-    <row r="93" spans="1:17">
-      <c r="A93" s="26"/>
-      <c r="B93" s="26"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="26"/>
-      <c r="H93" s="63"/>
-      <c r="I93" s="63"/>
-      <c r="J93" s="63"/>
-      <c r="K93" s="63"/>
-      <c r="L93" s="63"/>
-      <c r="M93" s="63"/>
-      <c r="N93" s="63"/>
-      <c r="O93" s="63"/>
-      <c r="P93" s="63"/>
-      <c r="Q93" s="63"/>
-    </row>
-    <row r="94" spans="1:17">
-      <c r="A94" s="26"/>
-      <c r="B94" s="26"/>
-      <c r="C94" s="26"/>
-      <c r="D94" s="26"/>
-      <c r="H94" s="63"/>
-      <c r="I94" s="63"/>
-      <c r="J94" s="63"/>
-      <c r="K94" s="63"/>
-      <c r="L94" s="63"/>
-      <c r="M94" s="63"/>
-      <c r="N94" s="63"/>
-      <c r="O94" s="63"/>
-      <c r="P94" s="63"/>
-      <c r="Q94" s="63"/>
-    </row>
-    <row r="95" spans="1:17">
-      <c r="A95" s="26"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="26"/>
-      <c r="H95" s="63"/>
-      <c r="I95" s="63"/>
-      <c r="J95" s="63"/>
-      <c r="K95" s="63"/>
-      <c r="L95" s="63"/>
-      <c r="M95" s="63"/>
-      <c r="N95" s="63"/>
-      <c r="O95" s="63"/>
-      <c r="P95" s="63"/>
-      <c r="Q95" s="63"/>
-    </row>
-    <row r="96" spans="1:17">
-      <c r="A96" s="26"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
-      <c r="D96" s="26"/>
-      <c r="H96" s="63"/>
-      <c r="I96" s="63"/>
-      <c r="J96" s="63"/>
-      <c r="K96" s="63"/>
-      <c r="L96" s="63"/>
-      <c r="M96" s="63"/>
-      <c r="N96" s="63"/>
-      <c r="O96" s="63"/>
-      <c r="P96" s="63"/>
-      <c r="Q96" s="63"/>
-    </row>
-    <row r="97" spans="1:17">
-      <c r="A97" s="26"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="26"/>
-      <c r="H97" s="63"/>
-      <c r="I97" s="63"/>
-      <c r="J97" s="63"/>
-      <c r="K97" s="63"/>
-      <c r="L97" s="63"/>
-      <c r="M97" s="63"/>
-      <c r="N97" s="63"/>
-      <c r="O97" s="63"/>
-      <c r="P97" s="63"/>
-      <c r="Q97" s="63"/>
-    </row>
-    <row r="98" spans="1:17">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="26"/>
-      <c r="D98" s="26"/>
-      <c r="H98" s="63"/>
-      <c r="I98" s="63"/>
-      <c r="J98" s="63"/>
-      <c r="K98" s="63"/>
-      <c r="L98" s="63"/>
-      <c r="M98" s="63"/>
-      <c r="N98" s="63"/>
-      <c r="O98" s="63"/>
-      <c r="P98" s="63"/>
-      <c r="Q98" s="63"/>
-    </row>
-    <row r="99" spans="1:17">
-      <c r="A99" s="26"/>
-      <c r="B99" s="26"/>
-      <c r="C99" s="26"/>
-      <c r="D99" s="26"/>
-      <c r="H99" s="63"/>
-      <c r="I99" s="63"/>
-      <c r="J99" s="63"/>
-      <c r="K99" s="63"/>
-      <c r="L99" s="63"/>
-      <c r="M99" s="63"/>
-      <c r="N99" s="63"/>
-      <c r="O99" s="63"/>
-      <c r="P99" s="63"/>
-      <c r="Q99" s="63"/>
-    </row>
-    <row r="100" spans="1:17">
-      <c r="A100" s="26"/>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
-      <c r="D100" s="26"/>
-      <c r="H100" s="63"/>
-      <c r="I100" s="63"/>
-      <c r="J100" s="63"/>
-      <c r="K100" s="63"/>
-      <c r="L100" s="63"/>
-      <c r="M100" s="63"/>
-      <c r="N100" s="63"/>
-      <c r="O100" s="63"/>
-      <c r="P100" s="63"/>
-      <c r="Q100" s="63"/>
-    </row>
-    <row r="101" spans="1:17">
-      <c r="A101" s="26"/>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
-      <c r="D101" s="26"/>
-      <c r="H101" s="63"/>
-      <c r="I101" s="63"/>
-      <c r="J101" s="63"/>
-      <c r="K101" s="63"/>
-      <c r="L101" s="63"/>
-      <c r="M101" s="63"/>
-      <c r="N101" s="63"/>
-      <c r="O101" s="63"/>
-      <c r="P101" s="63"/>
-      <c r="Q101" s="63"/>
-    </row>
-    <row r="102" spans="1:17">
-      <c r="A102" s="26"/>
-      <c r="B102" s="26"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="26"/>
-      <c r="H102" s="63"/>
-      <c r="I102" s="63"/>
-      <c r="J102" s="63"/>
-      <c r="K102" s="63"/>
-      <c r="L102" s="63"/>
-      <c r="M102" s="63"/>
-      <c r="N102" s="63"/>
-      <c r="O102" s="63"/>
-      <c r="P102" s="63"/>
-      <c r="Q102" s="63"/>
-    </row>
-    <row r="103" spans="1:17">
-      <c r="A103" s="26"/>
-      <c r="B103" s="26"/>
-      <c r="C103" s="26"/>
-      <c r="D103" s="26"/>
-      <c r="H103" s="63"/>
-      <c r="I103" s="63"/>
-      <c r="J103" s="63"/>
-      <c r="K103" s="63"/>
-      <c r="L103" s="63"/>
-      <c r="M103" s="63"/>
-      <c r="N103" s="63"/>
-      <c r="O103" s="63"/>
-      <c r="P103" s="63"/>
-      <c r="Q103" s="63"/>
-    </row>
-    <row r="104" spans="1:17">
-      <c r="A104" s="26"/>
-      <c r="B104" s="26"/>
-      <c r="C104" s="26"/>
-      <c r="D104" s="26"/>
-      <c r="H104" s="63"/>
-      <c r="I104" s="63"/>
-      <c r="J104" s="63"/>
-      <c r="K104" s="63"/>
-      <c r="L104" s="63"/>
-      <c r="M104" s="63"/>
-      <c r="N104" s="63"/>
-      <c r="O104" s="63"/>
-      <c r="P104" s="63"/>
-      <c r="Q104" s="63"/>
-    </row>
-    <row r="105" spans="1:17">
-      <c r="A105" s="26"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="26"/>
-      <c r="H105" s="63"/>
-      <c r="I105" s="63"/>
-      <c r="J105" s="63"/>
-      <c r="K105" s="63"/>
-      <c r="L105" s="63"/>
-      <c r="M105" s="63"/>
-      <c r="N105" s="63"/>
-      <c r="O105" s="63"/>
-      <c r="P105" s="63"/>
-      <c r="Q105" s="63"/>
-    </row>
-    <row r="106" spans="1:17">
-      <c r="A106" s="26"/>
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="H106" s="63"/>
-      <c r="I106" s="63"/>
-      <c r="J106" s="63"/>
-      <c r="K106" s="63"/>
-      <c r="L106" s="63"/>
-      <c r="M106" s="63"/>
-      <c r="N106" s="63"/>
-      <c r="O106" s="63"/>
-      <c r="P106" s="63"/>
-      <c r="Q106" s="63"/>
-    </row>
-    <row r="107" spans="1:17">
-      <c r="A107" s="26"/>
-      <c r="B107" s="26"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="26"/>
-      <c r="H107" s="63"/>
-      <c r="I107" s="63"/>
-      <c r="J107" s="63"/>
-      <c r="K107" s="63"/>
-      <c r="L107" s="63"/>
-      <c r="M107" s="63"/>
-      <c r="N107" s="63"/>
-      <c r="O107" s="63"/>
-      <c r="P107" s="63"/>
-      <c r="Q107" s="63"/>
-    </row>
-    <row r="108" spans="1:17">
-      <c r="A108" s="26"/>
-      <c r="B108" s="26"/>
-      <c r="C108" s="26"/>
-      <c r="D108" s="26"/>
-      <c r="H108" s="63"/>
-      <c r="I108" s="63"/>
-      <c r="J108" s="63"/>
-      <c r="K108" s="63"/>
-      <c r="L108" s="63"/>
-      <c r="M108" s="63"/>
-      <c r="N108" s="63"/>
-      <c r="O108" s="63"/>
-      <c r="P108" s="63"/>
-      <c r="Q108" s="63"/>
-    </row>
-    <row r="109" spans="1:17">
-      <c r="A109" s="26"/>
-      <c r="B109" s="26"/>
-      <c r="C109" s="26"/>
-      <c r="D109" s="26"/>
-      <c r="H109" s="63"/>
-      <c r="I109" s="63"/>
-      <c r="J109" s="63"/>
-      <c r="K109" s="63"/>
-      <c r="L109" s="63"/>
-      <c r="M109" s="63"/>
-      <c r="N109" s="63"/>
-      <c r="O109" s="63"/>
-      <c r="P109" s="63"/>
-      <c r="Q109" s="63"/>
-    </row>
-    <row r="110" spans="1:17">
-      <c r="A110" s="26"/>
-      <c r="B110" s="26"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="26"/>
-      <c r="H110" s="63"/>
-      <c r="I110" s="63"/>
-      <c r="J110" s="63"/>
-      <c r="K110" s="63"/>
-      <c r="L110" s="63"/>
-      <c r="M110" s="63"/>
-      <c r="N110" s="63"/>
-      <c r="O110" s="63"/>
-      <c r="P110" s="63"/>
-      <c r="Q110" s="63"/>
-    </row>
-    <row r="111" spans="1:17">
-      <c r="A111" s="26"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="26"/>
-      <c r="H111" s="63"/>
-      <c r="I111" s="63"/>
-      <c r="J111" s="63"/>
-      <c r="K111" s="63"/>
-      <c r="L111" s="63"/>
-      <c r="M111" s="63"/>
-      <c r="N111" s="63"/>
-      <c r="O111" s="63"/>
-      <c r="P111" s="63"/>
-      <c r="Q111" s="63"/>
-    </row>
-    <row r="112" spans="1:17">
-      <c r="A112" s="26"/>
-      <c r="B112" s="26"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="26"/>
-      <c r="H112" s="63"/>
-      <c r="I112" s="63"/>
-      <c r="J112" s="63"/>
-      <c r="K112" s="63"/>
-      <c r="L112" s="63"/>
-      <c r="M112" s="63"/>
-      <c r="N112" s="63"/>
-      <c r="O112" s="63"/>
-      <c r="P112" s="63"/>
-      <c r="Q112" s="63"/>
-    </row>
-    <row r="113" spans="1:17">
-      <c r="A113" s="26"/>
-      <c r="B113" s="26"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="26"/>
-      <c r="H113" s="63"/>
-      <c r="I113" s="63"/>
-      <c r="J113" s="63"/>
-      <c r="K113" s="63"/>
-      <c r="L113" s="63"/>
-      <c r="M113" s="63"/>
-      <c r="N113" s="63"/>
-      <c r="O113" s="63"/>
-      <c r="P113" s="63"/>
-      <c r="Q113" s="63"/>
-    </row>
-    <row r="114" spans="1:17">
-      <c r="A114" s="26"/>
-      <c r="B114" s="26"/>
-      <c r="C114" s="26"/>
-      <c r="D114" s="26"/>
-      <c r="H114" s="63"/>
-      <c r="I114" s="63"/>
-      <c r="J114" s="63"/>
-      <c r="K114" s="63"/>
-      <c r="L114" s="63"/>
-      <c r="M114" s="63"/>
-      <c r="N114" s="63"/>
-      <c r="O114" s="63"/>
-      <c r="P114" s="63"/>
-      <c r="Q114" s="63"/>
-    </row>
-    <row r="115" spans="1:17">
-      <c r="A115" s="26"/>
-      <c r="B115" s="26"/>
-      <c r="C115" s="26"/>
-      <c r="D115" s="26"/>
-      <c r="H115" s="63"/>
-      <c r="I115" s="63"/>
-      <c r="J115" s="63"/>
-      <c r="K115" s="63"/>
-      <c r="L115" s="63"/>
-      <c r="M115" s="63"/>
-      <c r="N115" s="63"/>
-      <c r="O115" s="63"/>
-      <c r="P115" s="63"/>
-      <c r="Q115" s="63"/>
-    </row>
-    <row r="116" spans="1:17">
-      <c r="A116" s="26"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="26"/>
-      <c r="D116" s="26"/>
-      <c r="H116" s="63"/>
-      <c r="I116" s="63"/>
-      <c r="J116" s="63"/>
-      <c r="K116" s="63"/>
-      <c r="L116" s="63"/>
-      <c r="M116" s="63"/>
-      <c r="N116" s="63"/>
-      <c r="O116" s="63"/>
-      <c r="P116" s="63"/>
-      <c r="Q116" s="63"/>
-    </row>
-    <row r="117" spans="1:17">
-      <c r="A117" s="26"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="26"/>
-      <c r="H117" s="63"/>
-      <c r="I117" s="63"/>
-      <c r="J117" s="63"/>
-      <c r="K117" s="63"/>
-      <c r="L117" s="63"/>
-      <c r="M117" s="63"/>
-      <c r="N117" s="63"/>
-      <c r="O117" s="63"/>
-      <c r="P117" s="63"/>
-      <c r="Q117" s="63"/>
-    </row>
-    <row r="118" spans="1:17">
-      <c r="A118" s="26"/>
-      <c r="B118" s="26"/>
-      <c r="C118" s="26"/>
-      <c r="D118" s="26"/>
-      <c r="H118" s="63"/>
-      <c r="I118" s="63"/>
-      <c r="J118" s="63"/>
-      <c r="K118" s="63"/>
-      <c r="L118" s="63"/>
-      <c r="M118" s="63"/>
-      <c r="N118" s="63"/>
-      <c r="O118" s="63"/>
-      <c r="P118" s="63"/>
-      <c r="Q118" s="63"/>
-    </row>
-    <row r="119" spans="1:17">
-      <c r="A119" s="26"/>
-      <c r="B119" s="26"/>
-      <c r="C119" s="26"/>
-      <c r="D119" s="26"/>
-      <c r="H119" s="63"/>
-      <c r="I119" s="63"/>
-      <c r="J119" s="63"/>
-      <c r="K119" s="63"/>
-      <c r="L119" s="63"/>
-      <c r="M119" s="63"/>
-      <c r="N119" s="63"/>
-      <c r="O119" s="63"/>
-      <c r="P119" s="63"/>
-      <c r="Q119" s="63"/>
-    </row>
-    <row r="120" spans="1:17">
-      <c r="A120" s="26"/>
-      <c r="B120" s="26"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="26"/>
-      <c r="H120" s="63"/>
-      <c r="I120" s="63"/>
-      <c r="J120" s="63"/>
-      <c r="K120" s="63"/>
-      <c r="L120" s="63"/>
-      <c r="M120" s="63"/>
-      <c r="N120" s="63"/>
-      <c r="O120" s="63"/>
-      <c r="P120" s="63"/>
-      <c r="Q120" s="63"/>
-    </row>
-    <row r="121" spans="1:17">
-      <c r="A121" s="26"/>
-      <c r="B121" s="26"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="26"/>
-      <c r="H121" s="63"/>
-      <c r="I121" s="63"/>
-      <c r="J121" s="63"/>
-      <c r="K121" s="63"/>
-      <c r="L121" s="63"/>
-      <c r="M121" s="63"/>
-      <c r="N121" s="63"/>
-      <c r="O121" s="63"/>
-      <c r="P121" s="63"/>
-      <c r="Q121" s="63"/>
-    </row>
-    <row r="122" spans="1:17">
-      <c r="A122" s="26"/>
-      <c r="B122" s="26"/>
-      <c r="C122" s="26"/>
-      <c r="D122" s="26"/>
-      <c r="H122" s="63"/>
-      <c r="I122" s="63"/>
-      <c r="J122" s="63"/>
-      <c r="K122" s="63"/>
-      <c r="L122" s="63"/>
-      <c r="M122" s="63"/>
-      <c r="N122" s="63"/>
-      <c r="O122" s="63"/>
-      <c r="P122" s="63"/>
-      <c r="Q122" s="63"/>
-    </row>
-    <row r="123" spans="1:17">
-      <c r="A123" s="26"/>
-      <c r="B123" s="26"/>
-      <c r="C123" s="26"/>
-      <c r="D123" s="26"/>
-      <c r="H123" s="63"/>
-      <c r="I123" s="63"/>
-      <c r="J123" s="63"/>
-      <c r="K123" s="63"/>
-      <c r="L123" s="63"/>
-      <c r="M123" s="63"/>
-      <c r="N123" s="63"/>
-      <c r="O123" s="63"/>
-      <c r="P123" s="63"/>
-      <c r="Q123" s="63"/>
-    </row>
-    <row r="124" spans="1:17">
-      <c r="A124" s="26"/>
-      <c r="B124" s="26"/>
-      <c r="C124" s="26"/>
-      <c r="D124" s="26"/>
-      <c r="H124" s="63"/>
-      <c r="I124" s="63"/>
-      <c r="J124" s="63"/>
-      <c r="K124" s="63"/>
-      <c r="L124" s="63"/>
-      <c r="M124" s="63"/>
-      <c r="N124" s="63"/>
-      <c r="O124" s="63"/>
-      <c r="P124" s="63"/>
-      <c r="Q124" s="63"/>
-    </row>
-    <row r="125" spans="1:17">
-      <c r="A125" s="26"/>
-      <c r="B125" s="26"/>
-      <c r="C125" s="26"/>
-      <c r="D125" s="26"/>
-      <c r="H125" s="63"/>
-      <c r="I125" s="63"/>
-      <c r="J125" s="63"/>
-      <c r="K125" s="63"/>
-      <c r="L125" s="63"/>
-      <c r="M125" s="63"/>
-      <c r="N125" s="63"/>
-      <c r="O125" s="63"/>
-      <c r="P125" s="63"/>
-      <c r="Q125" s="63"/>
+    <row r="93" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A93" s="48"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="53"/>
+      <c r="D93" s="50"/>
+      <c r="E93" s="51"/>
+      <c r="F93" s="51"/>
+      <c r="G93" s="51"/>
+      <c r="H93" s="72"/>
+      <c r="I93" s="72"/>
+      <c r="J93" s="73"/>
+      <c r="K93" s="72"/>
+      <c r="L93" s="72"/>
+      <c r="M93" s="74"/>
+      <c r="N93" s="74"/>
+      <c r="O93" s="74"/>
+      <c r="P93" s="74"/>
+      <c r="Q93" s="74"/>
+    </row>
+    <row r="94" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A94" s="48"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="53"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="51"/>
+      <c r="F94" s="51"/>
+      <c r="G94" s="51"/>
+      <c r="H94" s="72"/>
+      <c r="I94" s="72"/>
+      <c r="J94" s="73"/>
+      <c r="K94" s="72"/>
+      <c r="L94" s="72"/>
+      <c r="M94" s="74"/>
+      <c r="N94" s="74"/>
+      <c r="O94" s="74"/>
+      <c r="P94" s="74"/>
+      <c r="Q94" s="74"/>
+    </row>
+    <row r="95" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A95" s="48"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="53"/>
+      <c r="D95" s="50"/>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="72"/>
+      <c r="I95" s="72"/>
+      <c r="J95" s="73"/>
+      <c r="K95" s="72"/>
+      <c r="L95" s="72"/>
+      <c r="M95" s="74"/>
+      <c r="N95" s="74"/>
+      <c r="O95" s="74"/>
+      <c r="P95" s="74"/>
+      <c r="Q95" s="74"/>
+    </row>
+    <row r="96" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A96" s="48"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="53"/>
+      <c r="D96" s="50"/>
+      <c r="E96" s="51"/>
+      <c r="F96" s="51"/>
+      <c r="G96" s="51"/>
+      <c r="H96" s="72"/>
+      <c r="I96" s="72"/>
+      <c r="J96" s="73"/>
+      <c r="K96" s="72"/>
+      <c r="L96" s="72"/>
+      <c r="M96" s="74"/>
+      <c r="N96" s="74"/>
+      <c r="O96" s="74"/>
+      <c r="P96" s="74"/>
+      <c r="Q96" s="74"/>
+    </row>
+    <row r="97" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A97" s="48"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="53"/>
+      <c r="D97" s="50"/>
+      <c r="E97" s="51"/>
+      <c r="F97" s="51"/>
+      <c r="G97" s="51"/>
+      <c r="H97" s="72"/>
+      <c r="I97" s="72"/>
+      <c r="J97" s="73"/>
+      <c r="K97" s="72"/>
+      <c r="L97" s="72"/>
+      <c r="M97" s="74"/>
+      <c r="N97" s="74"/>
+      <c r="O97" s="74"/>
+      <c r="P97" s="74"/>
+      <c r="Q97" s="74"/>
+    </row>
+    <row r="98" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A98" s="48"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="53"/>
+      <c r="D98" s="50"/>
+      <c r="E98" s="51"/>
+      <c r="F98" s="51"/>
+      <c r="G98" s="51"/>
+      <c r="H98" s="72"/>
+      <c r="I98" s="72"/>
+      <c r="J98" s="73"/>
+      <c r="K98" s="72"/>
+      <c r="L98" s="72"/>
+      <c r="M98" s="74"/>
+      <c r="N98" s="74"/>
+      <c r="O98" s="74"/>
+      <c r="P98" s="74"/>
+      <c r="Q98" s="74"/>
+    </row>
+    <row r="99" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A99" s="48"/>
+      <c r="B99" s="49"/>
+      <c r="C99" s="53"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="51"/>
+      <c r="F99" s="51"/>
+      <c r="G99" s="51"/>
+      <c r="H99" s="72"/>
+      <c r="I99" s="72"/>
+      <c r="J99" s="73"/>
+      <c r="K99" s="72"/>
+      <c r="L99" s="72"/>
+      <c r="M99" s="74"/>
+      <c r="N99" s="74"/>
+      <c r="O99" s="74"/>
+      <c r="P99" s="74"/>
+      <c r="Q99" s="74"/>
+    </row>
+    <row r="100" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A100" s="48"/>
+      <c r="B100" s="49"/>
+      <c r="C100" s="53"/>
+      <c r="D100" s="50"/>
+      <c r="E100" s="51"/>
+      <c r="F100" s="51"/>
+      <c r="G100" s="51"/>
+      <c r="H100" s="72"/>
+      <c r="I100" s="72"/>
+      <c r="J100" s="73"/>
+      <c r="K100" s="72"/>
+      <c r="L100" s="72"/>
+      <c r="M100" s="74"/>
+      <c r="N100" s="74"/>
+      <c r="O100" s="74"/>
+      <c r="P100" s="74"/>
+      <c r="Q100" s="74"/>
+    </row>
+    <row r="101" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A101" s="48"/>
+      <c r="B101" s="49"/>
+      <c r="C101" s="53"/>
+      <c r="D101" s="50"/>
+      <c r="E101" s="51"/>
+      <c r="F101" s="51"/>
+      <c r="G101" s="51"/>
+      <c r="H101" s="72"/>
+      <c r="I101" s="72"/>
+      <c r="J101" s="73"/>
+      <c r="K101" s="72"/>
+      <c r="L101" s="72"/>
+      <c r="M101" s="74"/>
+      <c r="N101" s="74"/>
+      <c r="O101" s="74"/>
+      <c r="P101" s="74"/>
+      <c r="Q101" s="74"/>
+    </row>
+    <row r="102" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A102" s="48"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="53"/>
+      <c r="D102" s="50"/>
+      <c r="E102" s="51"/>
+      <c r="F102" s="51"/>
+      <c r="G102" s="51"/>
+      <c r="H102" s="72"/>
+      <c r="I102" s="72"/>
+      <c r="J102" s="73"/>
+      <c r="K102" s="72"/>
+      <c r="L102" s="72"/>
+      <c r="M102" s="74"/>
+      <c r="N102" s="74"/>
+      <c r="O102" s="74"/>
+      <c r="P102" s="74"/>
+      <c r="Q102" s="74"/>
+    </row>
+    <row r="103" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A103" s="48"/>
+      <c r="B103" s="49"/>
+      <c r="C103" s="53"/>
+      <c r="D103" s="50"/>
+      <c r="E103" s="51"/>
+      <c r="F103" s="51"/>
+      <c r="G103" s="51"/>
+      <c r="H103" s="72"/>
+      <c r="I103" s="72"/>
+      <c r="J103" s="73"/>
+      <c r="K103" s="72"/>
+      <c r="L103" s="72"/>
+      <c r="M103" s="74"/>
+      <c r="N103" s="74"/>
+      <c r="O103" s="74"/>
+      <c r="P103" s="74"/>
+      <c r="Q103" s="74"/>
+    </row>
+    <row r="104" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A104" s="48"/>
+      <c r="B104" s="49"/>
+      <c r="C104" s="53"/>
+      <c r="D104" s="50"/>
+      <c r="E104" s="51"/>
+      <c r="F104" s="51"/>
+      <c r="G104" s="51"/>
+      <c r="H104" s="72"/>
+      <c r="I104" s="72"/>
+      <c r="J104" s="73"/>
+      <c r="K104" s="72"/>
+      <c r="L104" s="72"/>
+      <c r="M104" s="74"/>
+      <c r="N104" s="74"/>
+      <c r="O104" s="74"/>
+      <c r="P104" s="74"/>
+      <c r="Q104" s="74"/>
+    </row>
+    <row r="105" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A105" s="48"/>
+      <c r="B105" s="49"/>
+      <c r="C105" s="53"/>
+      <c r="D105" s="50"/>
+      <c r="E105" s="51"/>
+      <c r="F105" s="51"/>
+      <c r="G105" s="51"/>
+      <c r="H105" s="72"/>
+      <c r="I105" s="72"/>
+      <c r="J105" s="73"/>
+      <c r="K105" s="72"/>
+      <c r="L105" s="72"/>
+      <c r="M105" s="74"/>
+      <c r="N105" s="74"/>
+      <c r="O105" s="74"/>
+      <c r="P105" s="74"/>
+      <c r="Q105" s="74"/>
+    </row>
+    <row r="106" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A106" s="48"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="53"/>
+      <c r="D106" s="50"/>
+      <c r="E106" s="51"/>
+      <c r="F106" s="51"/>
+      <c r="G106" s="51"/>
+      <c r="H106" s="72"/>
+      <c r="I106" s="72"/>
+      <c r="J106" s="73"/>
+      <c r="K106" s="72"/>
+      <c r="L106" s="72"/>
+      <c r="M106" s="74"/>
+      <c r="N106" s="74"/>
+      <c r="O106" s="74"/>
+      <c r="P106" s="74"/>
+      <c r="Q106" s="74"/>
+    </row>
+    <row r="107" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A107" s="48"/>
+      <c r="B107" s="49"/>
+      <c r="C107" s="53"/>
+      <c r="D107" s="50"/>
+      <c r="E107" s="51"/>
+      <c r="F107" s="51"/>
+      <c r="G107" s="51"/>
+      <c r="H107" s="72"/>
+      <c r="I107" s="72"/>
+      <c r="J107" s="73"/>
+      <c r="K107" s="72"/>
+      <c r="L107" s="72"/>
+      <c r="M107" s="74"/>
+      <c r="N107" s="74"/>
+      <c r="O107" s="74"/>
+      <c r="P107" s="74"/>
+      <c r="Q107" s="74"/>
+    </row>
+    <row r="108" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A108" s="48"/>
+      <c r="B108" s="49"/>
+      <c r="C108" s="53"/>
+      <c r="D108" s="50"/>
+      <c r="E108" s="51"/>
+      <c r="F108" s="51"/>
+      <c r="G108" s="51"/>
+      <c r="H108" s="72"/>
+      <c r="I108" s="72"/>
+      <c r="J108" s="73"/>
+      <c r="K108" s="72"/>
+      <c r="L108" s="72"/>
+      <c r="M108" s="74"/>
+      <c r="N108" s="74"/>
+      <c r="O108" s="74"/>
+      <c r="P108" s="74"/>
+      <c r="Q108" s="74"/>
+    </row>
+    <row r="109" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A109" s="48"/>
+      <c r="B109" s="49"/>
+      <c r="C109" s="53"/>
+      <c r="D109" s="50"/>
+      <c r="E109" s="51"/>
+      <c r="F109" s="51"/>
+      <c r="G109" s="51"/>
+      <c r="H109" s="72"/>
+      <c r="I109" s="72"/>
+      <c r="J109" s="73"/>
+      <c r="K109" s="72"/>
+      <c r="L109" s="72"/>
+      <c r="M109" s="74"/>
+      <c r="N109" s="74"/>
+      <c r="O109" s="74"/>
+      <c r="P109" s="74"/>
+      <c r="Q109" s="74"/>
+    </row>
+    <row r="110" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A110" s="48"/>
+      <c r="B110" s="49"/>
+      <c r="C110" s="53"/>
+      <c r="D110" s="50"/>
+      <c r="E110" s="51"/>
+      <c r="F110" s="51"/>
+      <c r="G110" s="51"/>
+      <c r="H110" s="72"/>
+      <c r="I110" s="72"/>
+      <c r="J110" s="73"/>
+      <c r="K110" s="72"/>
+      <c r="L110" s="72"/>
+      <c r="M110" s="74"/>
+      <c r="N110" s="74"/>
+      <c r="O110" s="74"/>
+      <c r="P110" s="74"/>
+      <c r="Q110" s="74"/>
+    </row>
+    <row r="111" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A111" s="48"/>
+      <c r="B111" s="49"/>
+      <c r="C111" s="53"/>
+      <c r="D111" s="50"/>
+      <c r="E111" s="51"/>
+      <c r="F111" s="51"/>
+      <c r="G111" s="51"/>
+      <c r="H111" s="72"/>
+      <c r="I111" s="72"/>
+      <c r="J111" s="73"/>
+      <c r="K111" s="72"/>
+      <c r="L111" s="72"/>
+      <c r="M111" s="74"/>
+      <c r="N111" s="74"/>
+      <c r="O111" s="74"/>
+      <c r="P111" s="74"/>
+      <c r="Q111" s="74"/>
+    </row>
+    <row r="112" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A112" s="48"/>
+      <c r="B112" s="49"/>
+      <c r="C112" s="53"/>
+      <c r="D112" s="50"/>
+      <c r="E112" s="51"/>
+      <c r="F112" s="51"/>
+      <c r="G112" s="51"/>
+      <c r="H112" s="72"/>
+      <c r="I112" s="72"/>
+      <c r="J112" s="73"/>
+      <c r="K112" s="72"/>
+      <c r="L112" s="72"/>
+      <c r="M112" s="74"/>
+      <c r="N112" s="74"/>
+      <c r="O112" s="74"/>
+      <c r="P112" s="74"/>
+      <c r="Q112" s="74"/>
+    </row>
+    <row r="113" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A113" s="48"/>
+      <c r="B113" s="49"/>
+      <c r="C113" s="53"/>
+      <c r="D113" s="50"/>
+      <c r="E113" s="51"/>
+      <c r="F113" s="51"/>
+      <c r="G113" s="51"/>
+      <c r="H113" s="72"/>
+      <c r="I113" s="72"/>
+      <c r="J113" s="73"/>
+      <c r="K113" s="72"/>
+      <c r="L113" s="72"/>
+      <c r="M113" s="74"/>
+      <c r="N113" s="74"/>
+      <c r="O113" s="74"/>
+      <c r="P113" s="74"/>
+      <c r="Q113" s="74"/>
+    </row>
+    <row r="114" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A114" s="48"/>
+      <c r="B114" s="49"/>
+      <c r="C114" s="53"/>
+      <c r="D114" s="50"/>
+      <c r="E114" s="51"/>
+      <c r="F114" s="51"/>
+      <c r="G114" s="51"/>
+      <c r="H114" s="72"/>
+      <c r="I114" s="72"/>
+      <c r="J114" s="73"/>
+      <c r="K114" s="72"/>
+      <c r="L114" s="72"/>
+      <c r="M114" s="74"/>
+      <c r="N114" s="74"/>
+      <c r="O114" s="74"/>
+      <c r="P114" s="74"/>
+      <c r="Q114" s="74"/>
+    </row>
+    <row r="115" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A115" s="48"/>
+      <c r="B115" s="49"/>
+      <c r="C115" s="53"/>
+      <c r="D115" s="50"/>
+      <c r="E115" s="51"/>
+      <c r="F115" s="51"/>
+      <c r="G115" s="51"/>
+      <c r="H115" s="72"/>
+      <c r="I115" s="72"/>
+      <c r="J115" s="73"/>
+      <c r="K115" s="72"/>
+      <c r="L115" s="72"/>
+      <c r="M115" s="74"/>
+      <c r="N115" s="74"/>
+      <c r="O115" s="74"/>
+      <c r="P115" s="74"/>
+      <c r="Q115" s="74"/>
+    </row>
+    <row r="116" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A116" s="48"/>
+      <c r="B116" s="49"/>
+      <c r="C116" s="53"/>
+      <c r="D116" s="50"/>
+      <c r="E116" s="51"/>
+      <c r="F116" s="51"/>
+      <c r="G116" s="51"/>
+      <c r="H116" s="72"/>
+      <c r="I116" s="72"/>
+      <c r="J116" s="73"/>
+      <c r="K116" s="72"/>
+      <c r="L116" s="72"/>
+      <c r="M116" s="74"/>
+      <c r="N116" s="74"/>
+      <c r="O116" s="74"/>
+      <c r="P116" s="74"/>
+      <c r="Q116" s="74"/>
+    </row>
+    <row r="117" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A117" s="48"/>
+      <c r="B117" s="49"/>
+      <c r="C117" s="53"/>
+      <c r="D117" s="50"/>
+      <c r="E117" s="51"/>
+      <c r="F117" s="51"/>
+      <c r="G117" s="51"/>
+      <c r="H117" s="72"/>
+      <c r="I117" s="72"/>
+      <c r="J117" s="73"/>
+      <c r="K117" s="72"/>
+      <c r="L117" s="72"/>
+      <c r="M117" s="74"/>
+      <c r="N117" s="74"/>
+      <c r="O117" s="74"/>
+      <c r="P117" s="74"/>
+      <c r="Q117" s="74"/>
+    </row>
+    <row r="118" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A118" s="48"/>
+      <c r="B118" s="49"/>
+      <c r="C118" s="53"/>
+      <c r="D118" s="50"/>
+      <c r="E118" s="51"/>
+      <c r="F118" s="51"/>
+      <c r="G118" s="51"/>
+      <c r="H118" s="72"/>
+      <c r="I118" s="72"/>
+      <c r="J118" s="73"/>
+      <c r="K118" s="72"/>
+      <c r="L118" s="72"/>
+      <c r="M118" s="74"/>
+      <c r="N118" s="74"/>
+      <c r="O118" s="74"/>
+      <c r="P118" s="74"/>
+      <c r="Q118" s="74"/>
+    </row>
+    <row r="119" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A119" s="48"/>
+      <c r="B119" s="49"/>
+      <c r="C119" s="53"/>
+      <c r="D119" s="50"/>
+      <c r="E119" s="51"/>
+      <c r="F119" s="51"/>
+      <c r="G119" s="51"/>
+      <c r="H119" s="72"/>
+      <c r="I119" s="72"/>
+      <c r="J119" s="73"/>
+      <c r="K119" s="72"/>
+      <c r="L119" s="72"/>
+      <c r="M119" s="74"/>
+      <c r="N119" s="74"/>
+      <c r="O119" s="74"/>
+      <c r="P119" s="74"/>
+      <c r="Q119" s="74"/>
+    </row>
+    <row r="120" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A120" s="48"/>
+      <c r="B120" s="49"/>
+      <c r="C120" s="53"/>
+      <c r="D120" s="50"/>
+      <c r="E120" s="51"/>
+      <c r="F120" s="51"/>
+      <c r="G120" s="51"/>
+      <c r="H120" s="72"/>
+      <c r="I120" s="72"/>
+      <c r="J120" s="73"/>
+      <c r="K120" s="72"/>
+      <c r="L120" s="72"/>
+      <c r="M120" s="74"/>
+      <c r="N120" s="74"/>
+      <c r="O120" s="74"/>
+      <c r="P120" s="74"/>
+      <c r="Q120" s="74"/>
+    </row>
+    <row r="121" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A121" s="48"/>
+      <c r="B121" s="49"/>
+      <c r="C121" s="53"/>
+      <c r="D121" s="50"/>
+      <c r="E121" s="51"/>
+      <c r="F121" s="51"/>
+      <c r="G121" s="51"/>
+      <c r="H121" s="72"/>
+      <c r="I121" s="72"/>
+      <c r="J121" s="73"/>
+      <c r="K121" s="72"/>
+      <c r="L121" s="72"/>
+      <c r="M121" s="74"/>
+      <c r="N121" s="74"/>
+      <c r="O121" s="74"/>
+      <c r="P121" s="74"/>
+      <c r="Q121" s="74"/>
+    </row>
+    <row r="122" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A122" s="48"/>
+      <c r="B122" s="49"/>
+      <c r="C122" s="53"/>
+      <c r="D122" s="50"/>
+      <c r="E122" s="51"/>
+      <c r="F122" s="51"/>
+      <c r="G122" s="51"/>
+      <c r="H122" s="72"/>
+      <c r="I122" s="72"/>
+      <c r="J122" s="73"/>
+      <c r="K122" s="72"/>
+      <c r="L122" s="72"/>
+      <c r="M122" s="74"/>
+      <c r="N122" s="74"/>
+      <c r="O122" s="74"/>
+      <c r="P122" s="74"/>
+      <c r="Q122" s="74"/>
+    </row>
+    <row r="123" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A123" s="48"/>
+      <c r="B123" s="49"/>
+      <c r="C123" s="53"/>
+      <c r="D123" s="50"/>
+      <c r="E123" s="51"/>
+      <c r="F123" s="51"/>
+      <c r="G123" s="51"/>
+      <c r="H123" s="72"/>
+      <c r="I123" s="72"/>
+      <c r="J123" s="73"/>
+      <c r="K123" s="72"/>
+      <c r="L123" s="72"/>
+      <c r="M123" s="74"/>
+      <c r="N123" s="74"/>
+      <c r="O123" s="74"/>
+      <c r="P123" s="74"/>
+      <c r="Q123" s="74"/>
+    </row>
+    <row r="124" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A124" s="48"/>
+      <c r="B124" s="49"/>
+      <c r="C124" s="53"/>
+      <c r="D124" s="50"/>
+      <c r="E124" s="51"/>
+      <c r="F124" s="51"/>
+      <c r="G124" s="51"/>
+      <c r="H124" s="72"/>
+      <c r="I124" s="72"/>
+      <c r="J124" s="73"/>
+      <c r="K124" s="72"/>
+      <c r="L124" s="72"/>
+      <c r="M124" s="74"/>
+      <c r="N124" s="74"/>
+      <c r="O124" s="74"/>
+      <c r="P124" s="74"/>
+      <c r="Q124" s="74"/>
+    </row>
+    <row r="125" spans="1:17" ht="48.75" customHeight="1">
+      <c r="A125" s="48"/>
+      <c r="B125" s="49"/>
+      <c r="C125" s="53"/>
+      <c r="D125" s="50"/>
+      <c r="E125" s="51"/>
+      <c r="F125" s="51"/>
+      <c r="G125" s="51"/>
+      <c r="H125" s="72"/>
+      <c r="I125" s="72"/>
+      <c r="J125" s="73"/>
+      <c r="K125" s="72"/>
+      <c r="L125" s="72"/>
+      <c r="M125" s="74"/>
+      <c r="N125" s="74"/>
+      <c r="O125" s="74"/>
+      <c r="P125" s="74"/>
+      <c r="Q125" s="74"/>
     </row>
     <row r="126" spans="1:17">
       <c r="A126" s="26"/>
@@ -17091,18 +17190,18 @@
   <sheetViews>
     <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.875" style="1" customWidth="1"/>
-    <col min="5" max="7" width="15.375" style="1" customWidth="1"/>
-    <col min="8" max="16" width="13.375" style="3" customWidth="1"/>
-    <col min="17" max="17" width="10.75" style="3" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="15.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16" width="13.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" style="3" customWidth="1"/>
     <col min="18" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
@@ -18381,527 +18480,1138 @@
       <c r="P62" s="76"/>
       <c r="Q62" s="76"/>
     </row>
-    <row r="63" spans="1:17">
-      <c r="A63" s="26"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="H63" s="63"/>
-      <c r="I63" s="63"/>
-      <c r="J63" s="63"/>
-      <c r="K63" s="63"/>
-      <c r="L63" s="63"/>
-      <c r="M63" s="63"/>
-      <c r="N63" s="63"/>
-      <c r="O63" s="63"/>
-      <c r="P63" s="63"/>
-      <c r="Q63" s="63"/>
-    </row>
-    <row r="64" spans="1:17">
-      <c r="A64" s="26"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
-      <c r="H64" s="63"/>
-      <c r="I64" s="63"/>
-      <c r="J64" s="63"/>
-      <c r="K64" s="63"/>
-      <c r="L64" s="63"/>
-      <c r="M64" s="63"/>
-      <c r="N64" s="63"/>
-      <c r="O64" s="63"/>
-      <c r="P64" s="63"/>
-      <c r="Q64" s="63"/>
-    </row>
-    <row r="65" spans="1:17">
-      <c r="A65" s="26"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="H65" s="63"/>
-      <c r="I65" s="63"/>
-      <c r="J65" s="63"/>
-      <c r="K65" s="63"/>
-      <c r="L65" s="63"/>
-      <c r="M65" s="63"/>
-      <c r="N65" s="63"/>
-      <c r="O65" s="63"/>
-      <c r="P65" s="63"/>
-      <c r="Q65" s="63"/>
-    </row>
-    <row r="66" spans="1:17">
-      <c r="A66" s="26"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
-      <c r="H66" s="63"/>
-      <c r="I66" s="63"/>
-      <c r="J66" s="63"/>
-      <c r="K66" s="63"/>
-      <c r="L66" s="63"/>
-      <c r="M66" s="63"/>
-      <c r="N66" s="63"/>
-      <c r="O66" s="63"/>
-      <c r="P66" s="63"/>
-      <c r="Q66" s="63"/>
-    </row>
-    <row r="67" spans="1:17">
-      <c r="A67" s="26"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
-      <c r="H67" s="63"/>
-      <c r="I67" s="63"/>
-      <c r="J67" s="63"/>
-      <c r="K67" s="63"/>
-      <c r="L67" s="63"/>
-      <c r="M67" s="63"/>
-      <c r="N67" s="63"/>
-      <c r="O67" s="63"/>
-      <c r="P67" s="63"/>
-      <c r="Q67" s="63"/>
-    </row>
-    <row r="68" spans="1:17">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
-      <c r="H68" s="63"/>
-      <c r="I68" s="63"/>
-      <c r="J68" s="63"/>
-      <c r="K68" s="63"/>
-      <c r="L68" s="63"/>
-      <c r="M68" s="63"/>
-      <c r="N68" s="63"/>
-      <c r="O68" s="63"/>
-      <c r="P68" s="63"/>
-      <c r="Q68" s="63"/>
-    </row>
-    <row r="69" spans="1:17">
-      <c r="A69" s="26"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="26"/>
-      <c r="D69" s="26"/>
-      <c r="H69" s="63"/>
-      <c r="I69" s="63"/>
-      <c r="J69" s="63"/>
-      <c r="K69" s="63"/>
-      <c r="L69" s="63"/>
-      <c r="M69" s="63"/>
-      <c r="N69" s="63"/>
-      <c r="O69" s="63"/>
-      <c r="P69" s="63"/>
-      <c r="Q69" s="63"/>
-    </row>
-    <row r="70" spans="1:17">
-      <c r="A70" s="26"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="26"/>
-      <c r="H70" s="63"/>
-      <c r="I70" s="63"/>
-      <c r="J70" s="63"/>
-      <c r="K70" s="63"/>
-      <c r="L70" s="63"/>
-      <c r="M70" s="63"/>
-      <c r="N70" s="63"/>
-      <c r="O70" s="63"/>
-      <c r="P70" s="63"/>
-      <c r="Q70" s="63"/>
-    </row>
-    <row r="71" spans="1:17">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
-      <c r="H71" s="63"/>
-      <c r="I71" s="63"/>
-      <c r="J71" s="63"/>
-      <c r="K71" s="63"/>
-      <c r="L71" s="63"/>
-      <c r="M71" s="63"/>
-      <c r="N71" s="63"/>
-      <c r="O71" s="63"/>
-      <c r="P71" s="63"/>
-      <c r="Q71" s="63"/>
-    </row>
-    <row r="72" spans="1:17">
-      <c r="A72" s="26"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
-      <c r="H72" s="63"/>
-      <c r="I72" s="63"/>
-      <c r="J72" s="63"/>
-      <c r="K72" s="63"/>
-      <c r="L72" s="63"/>
-      <c r="M72" s="63"/>
-      <c r="N72" s="63"/>
-      <c r="O72" s="63"/>
-      <c r="P72" s="63"/>
-      <c r="Q72" s="63"/>
-    </row>
-    <row r="73" spans="1:17">
-      <c r="A73" s="26"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
-      <c r="H73" s="63"/>
-      <c r="I73" s="63"/>
-      <c r="J73" s="63"/>
-      <c r="K73" s="63"/>
-      <c r="L73" s="63"/>
-      <c r="M73" s="63"/>
-      <c r="N73" s="63"/>
-      <c r="O73" s="63"/>
-      <c r="P73" s="63"/>
-      <c r="Q73" s="63"/>
-    </row>
-    <row r="74" spans="1:17">
-      <c r="A74" s="26"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-      <c r="H74" s="63"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="63"/>
-      <c r="K74" s="63"/>
-      <c r="L74" s="63"/>
-      <c r="M74" s="63"/>
-      <c r="N74" s="63"/>
-      <c r="O74" s="63"/>
-      <c r="P74" s="63"/>
-      <c r="Q74" s="63"/>
-    </row>
-    <row r="75" spans="1:17">
-      <c r="A75" s="26"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
-      <c r="H75" s="63"/>
-      <c r="I75" s="63"/>
-      <c r="J75" s="63"/>
-      <c r="K75" s="63"/>
-      <c r="L75" s="63"/>
-      <c r="M75" s="63"/>
-      <c r="N75" s="63"/>
-      <c r="O75" s="63"/>
-      <c r="P75" s="63"/>
-      <c r="Q75" s="63"/>
-    </row>
-    <row r="76" spans="1:17">
-      <c r="A76" s="26"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-    </row>
-    <row r="77" spans="1:17">
-      <c r="A77" s="26"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
-    </row>
-    <row r="78" spans="1:17">
-      <c r="A78" s="26"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
-    </row>
-    <row r="79" spans="1:17">
-      <c r="A79" s="26"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="26"/>
-    </row>
-    <row r="80" spans="1:17">
-      <c r="A80" s="26"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26"/>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="26"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="26"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="26"/>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="26"/>
-      <c r="B83" s="26"/>
-      <c r="C83" s="26"/>
-      <c r="D83" s="26"/>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="26"/>
-      <c r="B84" s="26"/>
-      <c r="C84" s="26"/>
-      <c r="D84" s="26"/>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="26"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="26"/>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="26"/>
-      <c r="B86" s="26"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="26"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="26"/>
-      <c r="B88" s="26"/>
-      <c r="C88" s="26"/>
-      <c r="D88" s="26"/>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="26"/>
-      <c r="B89" s="26"/>
-      <c r="C89" s="26"/>
-      <c r="D89" s="26"/>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="26"/>
-      <c r="B90" s="26"/>
-      <c r="C90" s="26"/>
-      <c r="D90" s="26"/>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="26"/>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="26"/>
-      <c r="B92" s="26"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="26"/>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="26"/>
-      <c r="B93" s="26"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="26"/>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="26"/>
-      <c r="B94" s="26"/>
-      <c r="C94" s="26"/>
-      <c r="D94" s="26"/>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="26"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="26"/>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="26"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
-      <c r="D96" s="26"/>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="26"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="26"/>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="26"/>
-      <c r="D98" s="26"/>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="26"/>
-      <c r="B99" s="26"/>
-      <c r="C99" s="26"/>
-      <c r="D99" s="26"/>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="26"/>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
-      <c r="D100" s="26"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="26"/>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
-      <c r="D101" s="26"/>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="26"/>
-      <c r="B102" s="26"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="26"/>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="26"/>
-      <c r="B103" s="26"/>
-      <c r="C103" s="26"/>
-      <c r="D103" s="26"/>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="26"/>
-      <c r="B104" s="26"/>
-      <c r="C104" s="26"/>
-      <c r="D104" s="26"/>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="26"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="26"/>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="26"/>
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="26"/>
-      <c r="B107" s="26"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="26"/>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="26"/>
-      <c r="B108" s="26"/>
-      <c r="C108" s="26"/>
-      <c r="D108" s="26"/>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="26"/>
-      <c r="B109" s="26"/>
-      <c r="C109" s="26"/>
-      <c r="D109" s="26"/>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="26"/>
-      <c r="B110" s="26"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="26"/>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="26"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="26"/>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="26"/>
-      <c r="B112" s="26"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="26"/>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="26"/>
-      <c r="B113" s="26"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="26"/>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="26"/>
-      <c r="B114" s="26"/>
-      <c r="C114" s="26"/>
-      <c r="D114" s="26"/>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="26"/>
-      <c r="B115" s="26"/>
-      <c r="C115" s="26"/>
-      <c r="D115" s="26"/>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="26"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="26"/>
-      <c r="D116" s="26"/>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="26"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="26"/>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="26"/>
-      <c r="B118" s="26"/>
-      <c r="C118" s="26"/>
-      <c r="D118" s="26"/>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="26"/>
-      <c r="B119" s="26"/>
-      <c r="C119" s="26"/>
-      <c r="D119" s="26"/>
-    </row>
-    <row r="120" spans="1:4">
+    <row r="63" spans="1:17" ht="48" customHeight="1">
+      <c r="A63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="51"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="77"/>
+      <c r="I63" s="77"/>
+      <c r="J63" s="75"/>
+      <c r="K63" s="75"/>
+      <c r="L63" s="75"/>
+      <c r="M63" s="76"/>
+      <c r="N63" s="76"/>
+      <c r="O63" s="76"/>
+      <c r="P63" s="76"/>
+      <c r="Q63" s="76"/>
+    </row>
+    <row r="64" spans="1:17" ht="48" customHeight="1">
+      <c r="A64" s="48"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="53"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="51"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="77"/>
+      <c r="I64" s="77"/>
+      <c r="J64" s="75"/>
+      <c r="K64" s="75"/>
+      <c r="L64" s="75"/>
+      <c r="M64" s="76"/>
+      <c r="N64" s="76"/>
+      <c r="O64" s="76"/>
+      <c r="P64" s="76"/>
+      <c r="Q64" s="76"/>
+    </row>
+    <row r="65" spans="1:17" ht="48" customHeight="1">
+      <c r="A65" s="48"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="51"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="77"/>
+      <c r="I65" s="77"/>
+      <c r="J65" s="75"/>
+      <c r="K65" s="75"/>
+      <c r="L65" s="75"/>
+      <c r="M65" s="76"/>
+      <c r="N65" s="76"/>
+      <c r="O65" s="76"/>
+      <c r="P65" s="76"/>
+      <c r="Q65" s="76"/>
+    </row>
+    <row r="66" spans="1:17" ht="48" customHeight="1">
+      <c r="A66" s="48"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="53"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="77"/>
+      <c r="I66" s="77"/>
+      <c r="J66" s="75"/>
+      <c r="K66" s="75"/>
+      <c r="L66" s="75"/>
+      <c r="M66" s="76"/>
+      <c r="N66" s="76"/>
+      <c r="O66" s="76"/>
+      <c r="P66" s="76"/>
+      <c r="Q66" s="76"/>
+    </row>
+    <row r="67" spans="1:17" ht="48" customHeight="1">
+      <c r="A67" s="48"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="53"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="77"/>
+      <c r="I67" s="77"/>
+      <c r="J67" s="75"/>
+      <c r="K67" s="75"/>
+      <c r="L67" s="75"/>
+      <c r="M67" s="76"/>
+      <c r="N67" s="76"/>
+      <c r="O67" s="76"/>
+      <c r="P67" s="76"/>
+      <c r="Q67" s="76"/>
+    </row>
+    <row r="68" spans="1:17" ht="48" customHeight="1">
+      <c r="A68" s="48"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="77"/>
+      <c r="I68" s="77"/>
+      <c r="J68" s="75"/>
+      <c r="K68" s="75"/>
+      <c r="L68" s="75"/>
+      <c r="M68" s="76"/>
+      <c r="N68" s="76"/>
+      <c r="O68" s="76"/>
+      <c r="P68" s="76"/>
+      <c r="Q68" s="76"/>
+    </row>
+    <row r="69" spans="1:17" ht="48" customHeight="1">
+      <c r="A69" s="48"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="77"/>
+      <c r="I69" s="77"/>
+      <c r="J69" s="75"/>
+      <c r="K69" s="75"/>
+      <c r="L69" s="75"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="76"/>
+      <c r="O69" s="76"/>
+      <c r="P69" s="76"/>
+      <c r="Q69" s="76"/>
+    </row>
+    <row r="70" spans="1:17" ht="48" customHeight="1">
+      <c r="A70" s="48"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="51"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="77"/>
+      <c r="I70" s="77"/>
+      <c r="J70" s="75"/>
+      <c r="K70" s="75"/>
+      <c r="L70" s="75"/>
+      <c r="M70" s="76"/>
+      <c r="N70" s="76"/>
+      <c r="O70" s="76"/>
+      <c r="P70" s="76"/>
+      <c r="Q70" s="76"/>
+    </row>
+    <row r="71" spans="1:17" ht="48" customHeight="1">
+      <c r="A71" s="48"/>
+      <c r="B71" s="49"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="51"/>
+      <c r="F71" s="51"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="77"/>
+      <c r="I71" s="77"/>
+      <c r="J71" s="75"/>
+      <c r="K71" s="75"/>
+      <c r="L71" s="75"/>
+      <c r="M71" s="76"/>
+      <c r="N71" s="76"/>
+      <c r="O71" s="76"/>
+      <c r="P71" s="76"/>
+      <c r="Q71" s="76"/>
+    </row>
+    <row r="72" spans="1:17" ht="48" customHeight="1">
+      <c r="A72" s="48"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="77"/>
+      <c r="I72" s="77"/>
+      <c r="J72" s="75"/>
+      <c r="K72" s="75"/>
+      <c r="L72" s="75"/>
+      <c r="M72" s="76"/>
+      <c r="N72" s="76"/>
+      <c r="O72" s="76"/>
+      <c r="P72" s="76"/>
+      <c r="Q72" s="76"/>
+    </row>
+    <row r="73" spans="1:17" ht="48" customHeight="1">
+      <c r="A73" s="48"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="51"/>
+      <c r="F73" s="51"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="77"/>
+      <c r="I73" s="77"/>
+      <c r="J73" s="75"/>
+      <c r="K73" s="75"/>
+      <c r="L73" s="75"/>
+      <c r="M73" s="76"/>
+      <c r="N73" s="76"/>
+      <c r="O73" s="76"/>
+      <c r="P73" s="76"/>
+      <c r="Q73" s="76"/>
+    </row>
+    <row r="74" spans="1:17" ht="48" customHeight="1">
+      <c r="A74" s="48"/>
+      <c r="B74" s="49"/>
+      <c r="C74" s="53"/>
+      <c r="D74" s="50"/>
+      <c r="E74" s="51"/>
+      <c r="F74" s="51"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="77"/>
+      <c r="I74" s="77"/>
+      <c r="J74" s="75"/>
+      <c r="K74" s="75"/>
+      <c r="L74" s="75"/>
+      <c r="M74" s="76"/>
+      <c r="N74" s="76"/>
+      <c r="O74" s="76"/>
+      <c r="P74" s="76"/>
+      <c r="Q74" s="76"/>
+    </row>
+    <row r="75" spans="1:17" ht="48" customHeight="1">
+      <c r="A75" s="48"/>
+      <c r="B75" s="49"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="51"/>
+      <c r="F75" s="51"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="77"/>
+      <c r="I75" s="77"/>
+      <c r="J75" s="75"/>
+      <c r="K75" s="75"/>
+      <c r="L75" s="75"/>
+      <c r="M75" s="76"/>
+      <c r="N75" s="76"/>
+      <c r="O75" s="76"/>
+      <c r="P75" s="76"/>
+      <c r="Q75" s="76"/>
+    </row>
+    <row r="76" spans="1:17" ht="48" customHeight="1">
+      <c r="A76" s="48"/>
+      <c r="B76" s="49"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="77"/>
+      <c r="I76" s="77"/>
+      <c r="J76" s="75"/>
+      <c r="K76" s="75"/>
+      <c r="L76" s="75"/>
+      <c r="M76" s="76"/>
+      <c r="N76" s="76"/>
+      <c r="O76" s="76"/>
+      <c r="P76" s="76"/>
+      <c r="Q76" s="76"/>
+    </row>
+    <row r="77" spans="1:17" ht="48" customHeight="1">
+      <c r="A77" s="48"/>
+      <c r="B77" s="49"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="51"/>
+      <c r="F77" s="51"/>
+      <c r="G77" s="51"/>
+      <c r="H77" s="77"/>
+      <c r="I77" s="77"/>
+      <c r="J77" s="75"/>
+      <c r="K77" s="75"/>
+      <c r="L77" s="75"/>
+      <c r="M77" s="76"/>
+      <c r="N77" s="76"/>
+      <c r="O77" s="76"/>
+      <c r="P77" s="76"/>
+      <c r="Q77" s="76"/>
+    </row>
+    <row r="78" spans="1:17" ht="48" customHeight="1">
+      <c r="A78" s="48"/>
+      <c r="B78" s="49"/>
+      <c r="C78" s="53"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="51"/>
+      <c r="F78" s="51"/>
+      <c r="G78" s="51"/>
+      <c r="H78" s="77"/>
+      <c r="I78" s="77"/>
+      <c r="J78" s="75"/>
+      <c r="K78" s="75"/>
+      <c r="L78" s="75"/>
+      <c r="M78" s="76"/>
+      <c r="N78" s="76"/>
+      <c r="O78" s="76"/>
+      <c r="P78" s="76"/>
+      <c r="Q78" s="76"/>
+    </row>
+    <row r="79" spans="1:17" ht="48" customHeight="1">
+      <c r="A79" s="48"/>
+      <c r="B79" s="49"/>
+      <c r="C79" s="53"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="51"/>
+      <c r="F79" s="51"/>
+      <c r="G79" s="51"/>
+      <c r="H79" s="77"/>
+      <c r="I79" s="77"/>
+      <c r="J79" s="75"/>
+      <c r="K79" s="75"/>
+      <c r="L79" s="75"/>
+      <c r="M79" s="76"/>
+      <c r="N79" s="76"/>
+      <c r="O79" s="76"/>
+      <c r="P79" s="76"/>
+      <c r="Q79" s="76"/>
+    </row>
+    <row r="80" spans="1:17" ht="48" customHeight="1">
+      <c r="A80" s="48"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="53"/>
+      <c r="D80" s="50"/>
+      <c r="E80" s="51"/>
+      <c r="F80" s="51"/>
+      <c r="G80" s="51"/>
+      <c r="H80" s="77"/>
+      <c r="I80" s="77"/>
+      <c r="J80" s="75"/>
+      <c r="K80" s="75"/>
+      <c r="L80" s="75"/>
+      <c r="M80" s="76"/>
+      <c r="N80" s="76"/>
+      <c r="O80" s="76"/>
+      <c r="P80" s="76"/>
+      <c r="Q80" s="76"/>
+    </row>
+    <row r="81" spans="1:17" ht="48" customHeight="1">
+      <c r="A81" s="48"/>
+      <c r="B81" s="49"/>
+      <c r="C81" s="53"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="51"/>
+      <c r="F81" s="51"/>
+      <c r="G81" s="51"/>
+      <c r="H81" s="77"/>
+      <c r="I81" s="77"/>
+      <c r="J81" s="75"/>
+      <c r="K81" s="75"/>
+      <c r="L81" s="75"/>
+      <c r="M81" s="76"/>
+      <c r="N81" s="76"/>
+      <c r="O81" s="76"/>
+      <c r="P81" s="76"/>
+      <c r="Q81" s="76"/>
+    </row>
+    <row r="82" spans="1:17" ht="48" customHeight="1">
+      <c r="A82" s="48"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="50"/>
+      <c r="E82" s="51"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="77"/>
+      <c r="I82" s="77"/>
+      <c r="J82" s="75"/>
+      <c r="K82" s="75"/>
+      <c r="L82" s="75"/>
+      <c r="M82" s="76"/>
+      <c r="N82" s="76"/>
+      <c r="O82" s="76"/>
+      <c r="P82" s="76"/>
+      <c r="Q82" s="76"/>
+    </row>
+    <row r="83" spans="1:17" ht="48" customHeight="1">
+      <c r="A83" s="48"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="53"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="51"/>
+      <c r="F83" s="51"/>
+      <c r="G83" s="51"/>
+      <c r="H83" s="77"/>
+      <c r="I83" s="77"/>
+      <c r="J83" s="75"/>
+      <c r="K83" s="75"/>
+      <c r="L83" s="75"/>
+      <c r="M83" s="76"/>
+      <c r="N83" s="76"/>
+      <c r="O83" s="76"/>
+      <c r="P83" s="76"/>
+      <c r="Q83" s="76"/>
+    </row>
+    <row r="84" spans="1:17" ht="48" customHeight="1">
+      <c r="A84" s="48"/>
+      <c r="B84" s="49"/>
+      <c r="C84" s="53"/>
+      <c r="D84" s="50"/>
+      <c r="E84" s="51"/>
+      <c r="F84" s="51"/>
+      <c r="G84" s="51"/>
+      <c r="H84" s="77"/>
+      <c r="I84" s="77"/>
+      <c r="J84" s="75"/>
+      <c r="K84" s="75"/>
+      <c r="L84" s="75"/>
+      <c r="M84" s="76"/>
+      <c r="N84" s="76"/>
+      <c r="O84" s="76"/>
+      <c r="P84" s="76"/>
+      <c r="Q84" s="76"/>
+    </row>
+    <row r="85" spans="1:17" ht="48" customHeight="1">
+      <c r="A85" s="48"/>
+      <c r="B85" s="49"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="50"/>
+      <c r="E85" s="51"/>
+      <c r="F85" s="51"/>
+      <c r="G85" s="51"/>
+      <c r="H85" s="77"/>
+      <c r="I85" s="77"/>
+      <c r="J85" s="75"/>
+      <c r="K85" s="75"/>
+      <c r="L85" s="75"/>
+      <c r="M85" s="76"/>
+      <c r="N85" s="76"/>
+      <c r="O85" s="76"/>
+      <c r="P85" s="76"/>
+      <c r="Q85" s="76"/>
+    </row>
+    <row r="86" spans="1:17" ht="48" customHeight="1">
+      <c r="A86" s="48"/>
+      <c r="B86" s="49"/>
+      <c r="C86" s="53"/>
+      <c r="D86" s="50"/>
+      <c r="E86" s="51"/>
+      <c r="F86" s="51"/>
+      <c r="G86" s="51"/>
+      <c r="H86" s="77"/>
+      <c r="I86" s="77"/>
+      <c r="J86" s="75"/>
+      <c r="K86" s="75"/>
+      <c r="L86" s="75"/>
+      <c r="M86" s="76"/>
+      <c r="N86" s="76"/>
+      <c r="O86" s="76"/>
+      <c r="P86" s="76"/>
+      <c r="Q86" s="76"/>
+    </row>
+    <row r="87" spans="1:17" ht="48" customHeight="1">
+      <c r="A87" s="48"/>
+      <c r="B87" s="49"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="50"/>
+      <c r="E87" s="51"/>
+      <c r="F87" s="51"/>
+      <c r="G87" s="51"/>
+      <c r="H87" s="77"/>
+      <c r="I87" s="77"/>
+      <c r="J87" s="75"/>
+      <c r="K87" s="75"/>
+      <c r="L87" s="75"/>
+      <c r="M87" s="76"/>
+      <c r="N87" s="76"/>
+      <c r="O87" s="76"/>
+      <c r="P87" s="76"/>
+      <c r="Q87" s="76"/>
+    </row>
+    <row r="88" spans="1:17" ht="48" customHeight="1">
+      <c r="A88" s="48"/>
+      <c r="B88" s="49"/>
+      <c r="C88" s="53"/>
+      <c r="D88" s="50"/>
+      <c r="E88" s="51"/>
+      <c r="F88" s="51"/>
+      <c r="G88" s="51"/>
+      <c r="H88" s="77"/>
+      <c r="I88" s="77"/>
+      <c r="J88" s="75"/>
+      <c r="K88" s="75"/>
+      <c r="L88" s="75"/>
+      <c r="M88" s="76"/>
+      <c r="N88" s="76"/>
+      <c r="O88" s="76"/>
+      <c r="P88" s="76"/>
+      <c r="Q88" s="76"/>
+    </row>
+    <row r="89" spans="1:17" ht="48" customHeight="1">
+      <c r="A89" s="48"/>
+      <c r="B89" s="49"/>
+      <c r="C89" s="53"/>
+      <c r="D89" s="50"/>
+      <c r="E89" s="51"/>
+      <c r="F89" s="51"/>
+      <c r="G89" s="51"/>
+      <c r="H89" s="77"/>
+      <c r="I89" s="77"/>
+      <c r="J89" s="75"/>
+      <c r="K89" s="75"/>
+      <c r="L89" s="75"/>
+      <c r="M89" s="76"/>
+      <c r="N89" s="76"/>
+      <c r="O89" s="76"/>
+      <c r="P89" s="76"/>
+      <c r="Q89" s="76"/>
+    </row>
+    <row r="90" spans="1:17" ht="48" customHeight="1">
+      <c r="A90" s="48"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="53"/>
+      <c r="D90" s="50"/>
+      <c r="E90" s="51"/>
+      <c r="F90" s="51"/>
+      <c r="G90" s="51"/>
+      <c r="H90" s="77"/>
+      <c r="I90" s="77"/>
+      <c r="J90" s="75"/>
+      <c r="K90" s="75"/>
+      <c r="L90" s="75"/>
+      <c r="M90" s="76"/>
+      <c r="N90" s="76"/>
+      <c r="O90" s="76"/>
+      <c r="P90" s="76"/>
+      <c r="Q90" s="76"/>
+    </row>
+    <row r="91" spans="1:17" ht="48" customHeight="1">
+      <c r="A91" s="48"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="53"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="51"/>
+      <c r="F91" s="51"/>
+      <c r="G91" s="51"/>
+      <c r="H91" s="77"/>
+      <c r="I91" s="77"/>
+      <c r="J91" s="75"/>
+      <c r="K91" s="75"/>
+      <c r="L91" s="75"/>
+      <c r="M91" s="76"/>
+      <c r="N91" s="76"/>
+      <c r="O91" s="76"/>
+      <c r="P91" s="76"/>
+      <c r="Q91" s="76"/>
+    </row>
+    <row r="92" spans="1:17" ht="48" customHeight="1">
+      <c r="A92" s="48"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="53"/>
+      <c r="D92" s="50"/>
+      <c r="E92" s="51"/>
+      <c r="F92" s="51"/>
+      <c r="G92" s="51"/>
+      <c r="H92" s="77"/>
+      <c r="I92" s="77"/>
+      <c r="J92" s="75"/>
+      <c r="K92" s="75"/>
+      <c r="L92" s="75"/>
+      <c r="M92" s="76"/>
+      <c r="N92" s="76"/>
+      <c r="O92" s="76"/>
+      <c r="P92" s="76"/>
+      <c r="Q92" s="76"/>
+    </row>
+    <row r="93" spans="1:17" ht="48" customHeight="1">
+      <c r="A93" s="48"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="53"/>
+      <c r="D93" s="50"/>
+      <c r="E93" s="51"/>
+      <c r="F93" s="51"/>
+      <c r="G93" s="51"/>
+      <c r="H93" s="77"/>
+      <c r="I93" s="77"/>
+      <c r="J93" s="75"/>
+      <c r="K93" s="75"/>
+      <c r="L93" s="75"/>
+      <c r="M93" s="76"/>
+      <c r="N93" s="76"/>
+      <c r="O93" s="76"/>
+      <c r="P93" s="76"/>
+      <c r="Q93" s="76"/>
+    </row>
+    <row r="94" spans="1:17" ht="48" customHeight="1">
+      <c r="A94" s="48"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="53"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="51"/>
+      <c r="F94" s="51"/>
+      <c r="G94" s="51"/>
+      <c r="H94" s="77"/>
+      <c r="I94" s="77"/>
+      <c r="J94" s="75"/>
+      <c r="K94" s="75"/>
+      <c r="L94" s="75"/>
+      <c r="M94" s="76"/>
+      <c r="N94" s="76"/>
+      <c r="O94" s="76"/>
+      <c r="P94" s="76"/>
+      <c r="Q94" s="76"/>
+    </row>
+    <row r="95" spans="1:17" ht="48" customHeight="1">
+      <c r="A95" s="48"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="53"/>
+      <c r="D95" s="50"/>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="77"/>
+      <c r="I95" s="77"/>
+      <c r="J95" s="75"/>
+      <c r="K95" s="75"/>
+      <c r="L95" s="75"/>
+      <c r="M95" s="76"/>
+      <c r="N95" s="76"/>
+      <c r="O95" s="76"/>
+      <c r="P95" s="76"/>
+      <c r="Q95" s="76"/>
+    </row>
+    <row r="96" spans="1:17" ht="48" customHeight="1">
+      <c r="A96" s="48"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="53"/>
+      <c r="D96" s="50"/>
+      <c r="E96" s="51"/>
+      <c r="F96" s="51"/>
+      <c r="G96" s="51"/>
+      <c r="H96" s="77"/>
+      <c r="I96" s="77"/>
+      <c r="J96" s="75"/>
+      <c r="K96" s="75"/>
+      <c r="L96" s="75"/>
+      <c r="M96" s="76"/>
+      <c r="N96" s="76"/>
+      <c r="O96" s="76"/>
+      <c r="P96" s="76"/>
+      <c r="Q96" s="76"/>
+    </row>
+    <row r="97" spans="1:17" ht="48" customHeight="1">
+      <c r="A97" s="48"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="53"/>
+      <c r="D97" s="50"/>
+      <c r="E97" s="51"/>
+      <c r="F97" s="51"/>
+      <c r="G97" s="51"/>
+      <c r="H97" s="77"/>
+      <c r="I97" s="77"/>
+      <c r="J97" s="75"/>
+      <c r="K97" s="75"/>
+      <c r="L97" s="75"/>
+      <c r="M97" s="76"/>
+      <c r="N97" s="76"/>
+      <c r="O97" s="76"/>
+      <c r="P97" s="76"/>
+      <c r="Q97" s="76"/>
+    </row>
+    <row r="98" spans="1:17" ht="48" customHeight="1">
+      <c r="A98" s="48"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="53"/>
+      <c r="D98" s="50"/>
+      <c r="E98" s="51"/>
+      <c r="F98" s="51"/>
+      <c r="G98" s="51"/>
+      <c r="H98" s="77"/>
+      <c r="I98" s="77"/>
+      <c r="J98" s="75"/>
+      <c r="K98" s="75"/>
+      <c r="L98" s="75"/>
+      <c r="M98" s="76"/>
+      <c r="N98" s="76"/>
+      <c r="O98" s="76"/>
+      <c r="P98" s="76"/>
+      <c r="Q98" s="76"/>
+    </row>
+    <row r="99" spans="1:17" ht="48" customHeight="1">
+      <c r="A99" s="48"/>
+      <c r="B99" s="49"/>
+      <c r="C99" s="53"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="51"/>
+      <c r="F99" s="51"/>
+      <c r="G99" s="51"/>
+      <c r="H99" s="77"/>
+      <c r="I99" s="77"/>
+      <c r="J99" s="75"/>
+      <c r="K99" s="75"/>
+      <c r="L99" s="75"/>
+      <c r="M99" s="76"/>
+      <c r="N99" s="76"/>
+      <c r="O99" s="76"/>
+      <c r="P99" s="76"/>
+      <c r="Q99" s="76"/>
+    </row>
+    <row r="100" spans="1:17" ht="48" customHeight="1">
+      <c r="A100" s="48"/>
+      <c r="B100" s="49"/>
+      <c r="C100" s="53"/>
+      <c r="D100" s="50"/>
+      <c r="E100" s="51"/>
+      <c r="F100" s="51"/>
+      <c r="G100" s="51"/>
+      <c r="H100" s="77"/>
+      <c r="I100" s="77"/>
+      <c r="J100" s="75"/>
+      <c r="K100" s="75"/>
+      <c r="L100" s="75"/>
+      <c r="M100" s="76"/>
+      <c r="N100" s="76"/>
+      <c r="O100" s="76"/>
+      <c r="P100" s="76"/>
+      <c r="Q100" s="76"/>
+    </row>
+    <row r="101" spans="1:17" ht="48" customHeight="1">
+      <c r="A101" s="48"/>
+      <c r="B101" s="49"/>
+      <c r="C101" s="53"/>
+      <c r="D101" s="50"/>
+      <c r="E101" s="51"/>
+      <c r="F101" s="51"/>
+      <c r="G101" s="51"/>
+      <c r="H101" s="77"/>
+      <c r="I101" s="77"/>
+      <c r="J101" s="75"/>
+      <c r="K101" s="75"/>
+      <c r="L101" s="75"/>
+      <c r="M101" s="76"/>
+      <c r="N101" s="76"/>
+      <c r="O101" s="76"/>
+      <c r="P101" s="76"/>
+      <c r="Q101" s="76"/>
+    </row>
+    <row r="102" spans="1:17" ht="48" customHeight="1">
+      <c r="A102" s="48"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="53"/>
+      <c r="D102" s="50"/>
+      <c r="E102" s="51"/>
+      <c r="F102" s="51"/>
+      <c r="G102" s="51"/>
+      <c r="H102" s="77"/>
+      <c r="I102" s="77"/>
+      <c r="J102" s="75"/>
+      <c r="K102" s="75"/>
+      <c r="L102" s="75"/>
+      <c r="M102" s="76"/>
+      <c r="N102" s="76"/>
+      <c r="O102" s="76"/>
+      <c r="P102" s="76"/>
+      <c r="Q102" s="76"/>
+    </row>
+    <row r="103" spans="1:17" ht="48" customHeight="1">
+      <c r="A103" s="48"/>
+      <c r="B103" s="49"/>
+      <c r="C103" s="53"/>
+      <c r="D103" s="50"/>
+      <c r="E103" s="51"/>
+      <c r="F103" s="51"/>
+      <c r="G103" s="51"/>
+      <c r="H103" s="77"/>
+      <c r="I103" s="77"/>
+      <c r="J103" s="75"/>
+      <c r="K103" s="75"/>
+      <c r="L103" s="75"/>
+      <c r="M103" s="76"/>
+      <c r="N103" s="76"/>
+      <c r="O103" s="76"/>
+      <c r="P103" s="76"/>
+      <c r="Q103" s="76"/>
+    </row>
+    <row r="104" spans="1:17" ht="48" customHeight="1">
+      <c r="A104" s="48"/>
+      <c r="B104" s="49"/>
+      <c r="C104" s="53"/>
+      <c r="D104" s="50"/>
+      <c r="E104" s="51"/>
+      <c r="F104" s="51"/>
+      <c r="G104" s="51"/>
+      <c r="H104" s="77"/>
+      <c r="I104" s="77"/>
+      <c r="J104" s="75"/>
+      <c r="K104" s="75"/>
+      <c r="L104" s="75"/>
+      <c r="M104" s="76"/>
+      <c r="N104" s="76"/>
+      <c r="O104" s="76"/>
+      <c r="P104" s="76"/>
+      <c r="Q104" s="76"/>
+    </row>
+    <row r="105" spans="1:17" ht="48" customHeight="1">
+      <c r="A105" s="48"/>
+      <c r="B105" s="49"/>
+      <c r="C105" s="53"/>
+      <c r="D105" s="50"/>
+      <c r="E105" s="51"/>
+      <c r="F105" s="51"/>
+      <c r="G105" s="51"/>
+      <c r="H105" s="77"/>
+      <c r="I105" s="77"/>
+      <c r="J105" s="75"/>
+      <c r="K105" s="75"/>
+      <c r="L105" s="75"/>
+      <c r="M105" s="76"/>
+      <c r="N105" s="76"/>
+      <c r="O105" s="76"/>
+      <c r="P105" s="76"/>
+      <c r="Q105" s="76"/>
+    </row>
+    <row r="106" spans="1:17" ht="48" customHeight="1">
+      <c r="A106" s="48"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="53"/>
+      <c r="D106" s="50"/>
+      <c r="E106" s="51"/>
+      <c r="F106" s="51"/>
+      <c r="G106" s="51"/>
+      <c r="H106" s="77"/>
+      <c r="I106" s="77"/>
+      <c r="J106" s="75"/>
+      <c r="K106" s="75"/>
+      <c r="L106" s="75"/>
+      <c r="M106" s="76"/>
+      <c r="N106" s="76"/>
+      <c r="O106" s="76"/>
+      <c r="P106" s="76"/>
+      <c r="Q106" s="76"/>
+    </row>
+    <row r="107" spans="1:17" ht="48" customHeight="1">
+      <c r="A107" s="48"/>
+      <c r="B107" s="49"/>
+      <c r="C107" s="53"/>
+      <c r="D107" s="50"/>
+      <c r="E107" s="51"/>
+      <c r="F107" s="51"/>
+      <c r="G107" s="51"/>
+      <c r="H107" s="77"/>
+      <c r="I107" s="77"/>
+      <c r="J107" s="75"/>
+      <c r="K107" s="75"/>
+      <c r="L107" s="75"/>
+      <c r="M107" s="76"/>
+      <c r="N107" s="76"/>
+      <c r="O107" s="76"/>
+      <c r="P107" s="76"/>
+      <c r="Q107" s="76"/>
+    </row>
+    <row r="108" spans="1:17" ht="48" customHeight="1">
+      <c r="A108" s="48"/>
+      <c r="B108" s="49"/>
+      <c r="C108" s="53"/>
+      <c r="D108" s="50"/>
+      <c r="E108" s="51"/>
+      <c r="F108" s="51"/>
+      <c r="G108" s="51"/>
+      <c r="H108" s="77"/>
+      <c r="I108" s="77"/>
+      <c r="J108" s="75"/>
+      <c r="K108" s="75"/>
+      <c r="L108" s="75"/>
+      <c r="M108" s="76"/>
+      <c r="N108" s="76"/>
+      <c r="O108" s="76"/>
+      <c r="P108" s="76"/>
+      <c r="Q108" s="76"/>
+    </row>
+    <row r="109" spans="1:17" ht="48" customHeight="1">
+      <c r="A109" s="48"/>
+      <c r="B109" s="49"/>
+      <c r="C109" s="53"/>
+      <c r="D109" s="50"/>
+      <c r="E109" s="51"/>
+      <c r="F109" s="51"/>
+      <c r="G109" s="51"/>
+      <c r="H109" s="77"/>
+      <c r="I109" s="77"/>
+      <c r="J109" s="75"/>
+      <c r="K109" s="75"/>
+      <c r="L109" s="75"/>
+      <c r="M109" s="76"/>
+      <c r="N109" s="76"/>
+      <c r="O109" s="76"/>
+      <c r="P109" s="76"/>
+      <c r="Q109" s="76"/>
+    </row>
+    <row r="110" spans="1:17" ht="48" customHeight="1">
+      <c r="A110" s="48"/>
+      <c r="B110" s="49"/>
+      <c r="C110" s="53"/>
+      <c r="D110" s="50"/>
+      <c r="E110" s="51"/>
+      <c r="F110" s="51"/>
+      <c r="G110" s="51"/>
+      <c r="H110" s="77"/>
+      <c r="I110" s="77"/>
+      <c r="J110" s="75"/>
+      <c r="K110" s="75"/>
+      <c r="L110" s="75"/>
+      <c r="M110" s="76"/>
+      <c r="N110" s="76"/>
+      <c r="O110" s="76"/>
+      <c r="P110" s="76"/>
+      <c r="Q110" s="76"/>
+    </row>
+    <row r="111" spans="1:17" ht="48" customHeight="1">
+      <c r="A111" s="48"/>
+      <c r="B111" s="49"/>
+      <c r="C111" s="53"/>
+      <c r="D111" s="50"/>
+      <c r="E111" s="51"/>
+      <c r="F111" s="51"/>
+      <c r="G111" s="51"/>
+      <c r="H111" s="77"/>
+      <c r="I111" s="77"/>
+      <c r="J111" s="75"/>
+      <c r="K111" s="75"/>
+      <c r="L111" s="75"/>
+      <c r="M111" s="76"/>
+      <c r="N111" s="76"/>
+      <c r="O111" s="76"/>
+      <c r="P111" s="76"/>
+      <c r="Q111" s="76"/>
+    </row>
+    <row r="112" spans="1:17" ht="48" customHeight="1">
+      <c r="A112" s="48"/>
+      <c r="B112" s="49"/>
+      <c r="C112" s="53"/>
+      <c r="D112" s="50"/>
+      <c r="E112" s="51"/>
+      <c r="F112" s="51"/>
+      <c r="G112" s="51"/>
+      <c r="H112" s="77"/>
+      <c r="I112" s="77"/>
+      <c r="J112" s="75"/>
+      <c r="K112" s="75"/>
+      <c r="L112" s="75"/>
+      <c r="M112" s="76"/>
+      <c r="N112" s="76"/>
+      <c r="O112" s="76"/>
+      <c r="P112" s="76"/>
+      <c r="Q112" s="76"/>
+    </row>
+    <row r="113" spans="1:17" ht="48" customHeight="1">
+      <c r="A113" s="48"/>
+      <c r="B113" s="49"/>
+      <c r="C113" s="53"/>
+      <c r="D113" s="50"/>
+      <c r="E113" s="51"/>
+      <c r="F113" s="51"/>
+      <c r="G113" s="51"/>
+      <c r="H113" s="77"/>
+      <c r="I113" s="77"/>
+      <c r="J113" s="75"/>
+      <c r="K113" s="75"/>
+      <c r="L113" s="75"/>
+      <c r="M113" s="76"/>
+      <c r="N113" s="76"/>
+      <c r="O113" s="76"/>
+      <c r="P113" s="76"/>
+      <c r="Q113" s="76"/>
+    </row>
+    <row r="114" spans="1:17" ht="48" customHeight="1">
+      <c r="A114" s="48"/>
+      <c r="B114" s="49"/>
+      <c r="C114" s="53"/>
+      <c r="D114" s="50"/>
+      <c r="E114" s="51"/>
+      <c r="F114" s="51"/>
+      <c r="G114" s="51"/>
+      <c r="H114" s="77"/>
+      <c r="I114" s="77"/>
+      <c r="J114" s="75"/>
+      <c r="K114" s="75"/>
+      <c r="L114" s="75"/>
+      <c r="M114" s="76"/>
+      <c r="N114" s="76"/>
+      <c r="O114" s="76"/>
+      <c r="P114" s="76"/>
+      <c r="Q114" s="76"/>
+    </row>
+    <row r="115" spans="1:17" ht="48" customHeight="1">
+      <c r="A115" s="48"/>
+      <c r="B115" s="49"/>
+      <c r="C115" s="53"/>
+      <c r="D115" s="50"/>
+      <c r="E115" s="51"/>
+      <c r="F115" s="51"/>
+      <c r="G115" s="51"/>
+      <c r="H115" s="77"/>
+      <c r="I115" s="77"/>
+      <c r="J115" s="75"/>
+      <c r="K115" s="75"/>
+      <c r="L115" s="75"/>
+      <c r="M115" s="76"/>
+      <c r="N115" s="76"/>
+      <c r="O115" s="76"/>
+      <c r="P115" s="76"/>
+      <c r="Q115" s="76"/>
+    </row>
+    <row r="116" spans="1:17" ht="48" customHeight="1">
+      <c r="A116" s="48"/>
+      <c r="B116" s="49"/>
+      <c r="C116" s="53"/>
+      <c r="D116" s="50"/>
+      <c r="E116" s="51"/>
+      <c r="F116" s="51"/>
+      <c r="G116" s="51"/>
+      <c r="H116" s="77"/>
+      <c r="I116" s="77"/>
+      <c r="J116" s="75"/>
+      <c r="K116" s="75"/>
+      <c r="L116" s="75"/>
+      <c r="M116" s="76"/>
+      <c r="N116" s="76"/>
+      <c r="O116" s="76"/>
+      <c r="P116" s="76"/>
+      <c r="Q116" s="76"/>
+    </row>
+    <row r="117" spans="1:17" ht="48" customHeight="1">
+      <c r="A117" s="48"/>
+      <c r="B117" s="49"/>
+      <c r="C117" s="53"/>
+      <c r="D117" s="50"/>
+      <c r="E117" s="51"/>
+      <c r="F117" s="51"/>
+      <c r="G117" s="51"/>
+      <c r="H117" s="77"/>
+      <c r="I117" s="77"/>
+      <c r="J117" s="75"/>
+      <c r="K117" s="75"/>
+      <c r="L117" s="75"/>
+      <c r="M117" s="76"/>
+      <c r="N117" s="76"/>
+      <c r="O117" s="76"/>
+      <c r="P117" s="76"/>
+      <c r="Q117" s="76"/>
+    </row>
+    <row r="118" spans="1:17" ht="48" customHeight="1">
+      <c r="A118" s="48"/>
+      <c r="B118" s="49"/>
+      <c r="C118" s="53"/>
+      <c r="D118" s="50"/>
+      <c r="E118" s="51"/>
+      <c r="F118" s="51"/>
+      <c r="G118" s="51"/>
+      <c r="H118" s="77"/>
+      <c r="I118" s="77"/>
+      <c r="J118" s="75"/>
+      <c r="K118" s="75"/>
+      <c r="L118" s="75"/>
+      <c r="M118" s="76"/>
+      <c r="N118" s="76"/>
+      <c r="O118" s="76"/>
+      <c r="P118" s="76"/>
+      <c r="Q118" s="76"/>
+    </row>
+    <row r="119" spans="1:17" ht="48" customHeight="1">
+      <c r="A119" s="48"/>
+      <c r="B119" s="49"/>
+      <c r="C119" s="53"/>
+      <c r="D119" s="50"/>
+      <c r="E119" s="51"/>
+      <c r="F119" s="51"/>
+      <c r="G119" s="51"/>
+      <c r="H119" s="77"/>
+      <c r="I119" s="77"/>
+      <c r="J119" s="75"/>
+      <c r="K119" s="75"/>
+      <c r="L119" s="75"/>
+      <c r="M119" s="76"/>
+      <c r="N119" s="76"/>
+      <c r="O119" s="76"/>
+      <c r="P119" s="76"/>
+      <c r="Q119" s="76"/>
+    </row>
+    <row r="120" spans="1:17">
       <c r="A120" s="26"/>
       <c r="B120" s="26"/>
       <c r="C120" s="26"/>
       <c r="D120" s="26"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:17">
       <c r="A121" s="26"/>
       <c r="B121" s="26"/>
       <c r="C121" s="26"/>
       <c r="D121" s="26"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:17">
       <c r="A122" s="26"/>
       <c r="B122" s="26"/>
       <c r="C122" s="26"/>
       <c r="D122" s="26"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:17">
       <c r="A123" s="26"/>
       <c r="B123" s="26"/>
       <c r="C123" s="26"/>
       <c r="D123" s="26"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:17">
       <c r="A124" s="26"/>
       <c r="B124" s="26"/>
       <c r="C124" s="26"/>
       <c r="D124" s="26"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:17">
       <c r="A125" s="26"/>
       <c r="B125" s="26"/>
       <c r="C125" s="26"/>
       <c r="D125" s="26"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:17">
       <c r="A126" s="26"/>
       <c r="B126" s="26"/>
       <c r="C126" s="26"/>
       <c r="D126" s="26"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:17">
       <c r="A127" s="26"/>
       <c r="B127" s="26"/>
       <c r="C127" s="26"/>
       <c r="D127" s="26"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:17">
       <c r="A128" s="26"/>
       <c r="B128" s="26"/>
       <c r="C128" s="26"/>

</xml_diff>